<commit_message>
Add initial distributed results
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Work\Desktop\JuliaPro Programs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c3ba8ffd848b52ee/Documents/MSU/Homework/CSE812/cse812-project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A3CF0CC-2458-4C95-8F10-339E13FA0D92}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="28" documentId="13_ncr:1_{0A3CF0CC-2458-4C95-8F10-339E13FA0D92}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{32A37BC9-8BC2-44C1-AAF6-24623D425C12}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-3120" windowWidth="29040" windowHeight="15840" xr2:uid="{B707807D-57EB-4A6E-B54E-2E3DFFBA463E}"/>
+    <workbookView xWindow="315" yWindow="345" windowWidth="28800" windowHeight="11385" activeTab="1" xr2:uid="{B707807D-57EB-4A6E-B54E-2E3DFFBA463E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>V</t>
   </si>
@@ -57,6 +58,21 @@
   </si>
   <si>
     <t>CPU Used: Intel i7-4710HQ @ 2.50GHz</t>
+  </si>
+  <si>
+    <t>Vertices</t>
+  </si>
+  <si>
+    <t>Edges</t>
+  </si>
+  <si>
+    <t>Time (ms)</t>
+  </si>
+  <si>
+    <t>Observation: Changing E has significant impact on runtime</t>
+  </si>
+  <si>
+    <t>CPU Used: Intel i7-6600K @ 4.00GHz</t>
   </si>
 </sst>
 </file>
@@ -187,6 +203,18 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{298A2AC4-01DE-4225-A609-AB4B6CAC2A7C}" name="Table1" displayName="Table1" ref="A1:C6" totalsRowShown="0">
+  <autoFilter ref="A1:C6" xr:uid="{2F927F47-5A92-497A-8371-FE04470D820E}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{83727206-4DB4-4592-9999-939511C2E10C}" name="Vertices"/>
+    <tableColumn id="2" xr3:uid="{84A97E09-148D-4E3D-8329-99995EE3E5A8}" name="Edges"/>
+    <tableColumn id="3" xr3:uid="{68B37ECB-0077-451F-BE99-FD2D6B0DF1F9}" name="Time (ms)"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -488,8 +516,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12B1E35D-17AB-4482-B94A-FF8557483234}">
   <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A30" sqref="A30:A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -881,4 +909,107 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{276D49D4-41D7-4F95-ADA9-A8804576B2A7}">
+  <dimension ref="A1:C11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.42578125" customWidth="1"/>
+    <col min="3" max="3" width="12" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>64</v>
+      </c>
+      <c r="B2">
+        <v>1000</v>
+      </c>
+      <c r="C2">
+        <v>6.6189999999999998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>128</v>
+      </c>
+      <c r="B3">
+        <v>4000</v>
+      </c>
+      <c r="C3">
+        <v>22.363</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>256</v>
+      </c>
+      <c r="B4">
+        <v>16000</v>
+      </c>
+      <c r="C4">
+        <v>86.311000000000007</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>512</v>
+      </c>
+      <c r="B5">
+        <v>64000</v>
+      </c>
+      <c r="C5">
+        <v>588.45699999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>512</v>
+      </c>
+      <c r="B6">
+        <v>128000</v>
+      </c>
+      <c r="C6">
+        <v>2348</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
update with results for distributed alg and graph
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c3ba8ffd848b52ee/Documents/MSU/Homework/CSE812/cse812-project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="28" documentId="13_ncr:1_{0A3CF0CC-2458-4C95-8F10-339E13FA0D92}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{32A37BC9-8BC2-44C1-AAF6-24623D425C12}"/>
+  <xr:revisionPtr revIDLastSave="48" documentId="13_ncr:1_{0A3CF0CC-2458-4C95-8F10-339E13FA0D92}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{2AA2D615-FF71-4193-9CF1-60221BF95572}"/>
   <bookViews>
-    <workbookView xWindow="315" yWindow="345" windowWidth="28800" windowHeight="11385" activeTab="1" xr2:uid="{B707807D-57EB-4A6E-B54E-2E3DFFBA463E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" activeTab="1" xr2:uid="{B707807D-57EB-4A6E-B54E-2E3DFFBA463E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -203,6 +203,1095 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Time (ms)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.11549431321084865"/>
+                  <c:y val="-0.13930555555555554"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$B$2:$B$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>64000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>128000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$C$2:$C$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>6.6189999999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>22.363</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>86.311000000000007</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>588.45699999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2348</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-995B-4C00-99A4-544EDCEDF437}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="748594576"/>
+        <c:axId val="435750960"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="748594576"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Number</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> of Edges</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="435750960"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="435750960"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>wall</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Time (ms)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="748594576"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>166687</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>552450</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>152401</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{37411020-85A9-42B2-BEC6-104A26C1A1DE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -915,8 +2004,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{276D49D4-41D7-4F95-ADA9-A8804576B2A7}">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="W15" sqref="W15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1008,8 +2097,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>